<commit_message>
update 20 mei 2023
</commit_message>
<xml_diff>
--- a/Perkiraan Penyelesaian Bab.xlsx
+++ b/Perkiraan Penyelesaian Bab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/semester 7/projectskripsi2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_37FD5514EDF0C2BF0D24928CF41E5DB75F93BF7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA884C19-6182-4950-A6B8-11DBB9F13381}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C70A5702-4048-4BFD-B38C-40F495F869FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4C970EC-5EF6-46F5-A5F8-15A6D5F97C81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,23 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>BIMBINGAN PER BAB</t>
   </si>
@@ -106,13 +117,61 @@
   </si>
   <si>
     <t>SEKOLAH TINGGI TEOLOGI HAPPY FAMILY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list pertanyaan : penelitian </t>
+  </si>
+  <si>
+    <t>Bagaimana Kajian Teologis 2 Petrus 1:5-7 ?</t>
+  </si>
+  <si>
+    <t>Apa itu Pertumbuhan Pengenalan Akan ALLAH ?</t>
+  </si>
+  <si>
+    <t>Bagaimana kajian teologis 2 Petrus 1:5-7 dan aplikasinya dalam pertumbuhan pengenalan akan ALLAH Di MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World ?</t>
+  </si>
+  <si>
+    <t>Menurut anda apa itu pertumbuhan pengenalan akan Allah ?</t>
+  </si>
+  <si>
+    <t>Apa saja faktor-faktor yang mempengaruhi Pertumbuhan Pengenalan akan Allah di kalangan anggota MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apa pendapat anda tentang 2 Petrus 1:5-7 ? Jelaskan </t>
+  </si>
+  <si>
+    <t>Menurut anda apa yang dimaksud dengan "bersungguh-sungguh" dan "menambahkan" dalam konteks 2 Petrus 1:5-7 ini ?</t>
+  </si>
+  <si>
+    <t>Bagaimana pemahaman akan 2 Petrus 1:5-7 dapat berkontribusi bagi kalangan anggota MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World ?</t>
+  </si>
+  <si>
+    <t>Bagaimana kualitas-kualitas yang disebutkan dalam 2 Petrus 1:5-7 (seperti iman, kebajikan, pengetahuan, penguasaan diri,kasih persaudaraan) dapat diterapkan dalam kehidupan sehari-hari bagi anggota MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World?</t>
+  </si>
+  <si>
+    <t>Apa saja karakteristik seorang yang dalam proses pertumbuhan pengenalan akan Allah ?</t>
+  </si>
+  <si>
+    <t>Bagaimana MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World mendukung dan mendorong anggotanya untuk mengalami pertumbuhan pengenalan akan Allah berdasarkan kajian teologis 2 Petrus 1:5-7 ?</t>
+  </si>
+  <si>
+    <t>Bagaimana mengevaluasi efektivitas pertumbuhan pengenalan akan Allah berdasarkan kajian teologis 2 Petrus 1:5-7 di kalangan MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World ?</t>
+  </si>
+  <si>
+    <t>Bagaimana partisipasi anggota MDC Youth GKPB Masa Depan Cerah Surabaya Ciputra World dalam kajian teologis 2 Petrus 1:5-7 mempengaruhi hubungan mereka dengan Allah dan satu sama lain ?</t>
+  </si>
+  <si>
+    <t>Bagaimana pemahaman dan pengalaman anggota MDC Youth GKPB Masa Depan Cerah  Surabaya Ciputra World terkait dengan kajian teologis 2 Petrus 1:5-7 perihal bertumbuh dan pengenalan akan Allah ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +192,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -407,6 +479,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -416,34 +531,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,34 +878,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="85.88671875" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
@@ -842,13 +937,13 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="27">
         <v>44947</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="27">
         <v>44956</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -858,8 +953,12 @@
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="28">
+        <v>45066</v>
+      </c>
+      <c r="E6" s="28">
+        <v>45066</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -869,8 +968,10 @@
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="28">
+        <v>45066</v>
+      </c>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -880,8 +981,8 @@
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -891,8 +992,8 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -902,76 +1003,160 @@
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="19" spans="2:8" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="13"/>
+      <c r="C21" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="13"/>
+      <c r="C22" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="13"/>
+      <c r="C24" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="13"/>
+      <c r="C25" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="13"/>
+      <c r="C26" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="13"/>
+      <c r="C28" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="13"/>
+      <c r="C29" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="13"/>
+      <c r="C30" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="B27:B30"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update 03 juli 2023
</commit_message>
<xml_diff>
--- a/Perkiraan Penyelesaian Bab.xlsx
+++ b/Perkiraan Penyelesaian Bab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/semester 7/projectskripsi2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C70A5702-4048-4BFD-B38C-40F495F869FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4C970EC-5EF6-46F5-A5F8-15A6D5F97C81}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{C70A5702-4048-4BFD-B38C-40F495F869FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2023684D-7160-47D4-BB0C-3723081FA0D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -489,6 +489,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -515,30 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,10 +557,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -598,9 +602,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,26 +637,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -685,26 +672,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -880,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,20 +863,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
@@ -937,10 +907,10 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="13">
         <v>44947</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="13">
         <v>44956</v>
       </c>
       <c r="G5" s="9"/>
@@ -953,10 +923,10 @@
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="14">
         <v>45066</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="14">
         <v>45066</v>
       </c>
     </row>
@@ -968,10 +938,12 @@
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="14">
         <v>45066</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="14">
+        <v>45070</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -981,8 +953,8 @@
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -992,8 +964,8 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -1003,74 +975,74 @@
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="19" spans="2:8" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -1078,19 +1050,19 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -1098,25 +1070,25 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="13"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -1124,36 +1096,36 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="13"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="11" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>